<commit_message>
this is my fourth commit
</commit_message>
<xml_diff>
--- a/testdata/userdata.xlsx
+++ b/testdata/userdata.xlsx
@@ -55,16 +55,16 @@
     <t>active</t>
   </si>
   <si>
-    <t>user111223qqghrttfggdedgg@x.com</t>
-  </si>
-  <si>
-    <t>user498988hhjkhjbkeerfre4rjj@a.com</t>
-  </si>
-  <si>
-    <t>user2345egdgfgfghrferfer4j@l.com</t>
-  </si>
-  <si>
-    <t>user32343948fdjjfhorfr4grfr5o@g.com</t>
+    <t>user111223qqghr23344ffy6dedg@x.com</t>
+  </si>
+  <si>
+    <t>user498988hhjkhjbke33333eee3jj@a.com</t>
+  </si>
+  <si>
+    <t>user32343948fdjj1234dfv5333o@g.com</t>
+  </si>
+  <si>
+    <t>user2345egdgfgfghrf4555ffff4e4j@l.com</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -456,7 +456,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -470,7 +470,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
this is my fifth commit
</commit_message>
<xml_diff>
--- a/testdata/userdata.xlsx
+++ b/testdata/userdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="12195" windowHeight="3345"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="4695"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>name</t>
   </si>
@@ -31,40 +30,28 @@
     <t>status</t>
   </si>
   <si>
-    <t>testuser1</t>
-  </si>
-  <si>
-    <t>Male</t>
+    <t>user_davisjames@123</t>
+  </si>
+  <si>
+    <t>user_scottstevy@456</t>
+  </si>
+  <si>
+    <t>stevewauhghg</t>
+  </si>
+  <si>
+    <t>janesgerde</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
   <si>
     <t>inactive</t>
   </si>
   <si>
-    <t>testuser2</t>
-  </si>
-  <si>
-    <t>testuser3</t>
-  </si>
-  <si>
-    <t>testuser4</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>active</t>
-  </si>
-  <si>
-    <t>user111223qqghr23344ffy6dedg@x.com</t>
-  </si>
-  <si>
-    <t>user498988hhjkhjbke33333eee3jj@a.com</t>
-  </si>
-  <si>
-    <t>user32343948fdjj1234dfv5333o@g.com</t>
-  </si>
-  <si>
-    <t>user2345egdgfgfghrf4555ffff4e4j@l.com</t>
   </si>
 </sst>
 </file>
@@ -409,18 +396,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="35.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -439,16 +426,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -456,49 +443,19 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B4" r:id="rId3"/>
-    <hyperlink ref="B5" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>